<commit_message>
Changes on Rest Assured
</commit_message>
<xml_diff>
--- a/restassured-api-framework-hemanth/src/test/resources/testdata/testData.xlsx
+++ b/restassured-api-framework-hemanth/src/test/resources/testdata/testData.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E53B17-A61A-834C-8E6F-2F8ED1343076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13340" yWindow="4080" windowWidth="16940" windowHeight="8000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13344" yWindow="4080" windowWidth="16944" windowHeight="8004"/>
   </bookViews>
   <sheets>
     <sheet name="createNewUserWithData" sheetId="2" r:id="rId1"/>
@@ -47,16 +46,16 @@
     <t>inactive</t>
   </si>
   <si>
-    <t>testemail5@email.com</t>
-  </si>
-  <si>
-    <t>testemail6@gmail.com</t>
+    <t>testemail7@gmail.com</t>
+  </si>
+  <si>
+    <t>testemail8@email.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -119,7 +118,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -161,7 +160,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -194,26 +193,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -246,23 +228,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -438,19 +403,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="24.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,12 +429,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -478,12 +443,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -494,8 +459,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{BB4C90B5-EE6C-6D4D-928C-83E43C98448F}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{EFDF4529-262D-4849-B47E-BE828C1109A3}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>